<commit_message>
script arma excel con endpoint 2019
</commit_message>
<xml_diff>
--- a/bin/Debug/net6.0/Resultados.xlsx
+++ b/bin/Debug/net6.0/Resultados.xlsx
@@ -12,36 +12,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>IdMesa</t>
+    <t>Mesa</t>
   </si>
   <si>
-    <t>NombreAgrupacion</t>
+    <t>Circuito</t>
   </si>
   <si>
-    <t>VotosNulos</t>
+    <t>Cantidad de Votantes</t>
   </si>
   <si>
-    <t>VotosNulosPorcentaje</t>
+    <t>FRENTE DE IZQUIERDA Y DE TRABAJADORES - UNIDAD</t>
   </si>
   <si>
-    <t>VotosEnBlanco</t>
+    <t>CONSENSO FEDERAL</t>
   </si>
   <si>
-    <t>VotosEnBlancoPorcentaje</t>
+    <t>JUNTOS POR EL CAMBIO</t>
   </si>
   <si>
-    <t>VotosRecurridosComandoImpugnados</t>
+    <t>FRENTE DE TODOS</t>
   </si>
   <si>
-    <t>VotosRecurridosComandoImpugnadosPorcentaje</t>
+    <t>UNITE POR LA LIBERTAD Y LA DIGNIDAD</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Votos Nulos</t>
+  </si>
+  <si>
+    <t>Votos Recurridos</t>
+  </si>
+  <si>
+    <t>Votos impugnados</t>
+  </si>
+  <si>
+    <t>Votos en blanco</t>
   </si>
   <si>
     <t>1244</t>
+  </si>
+  <si>
+    <t>00039</t>
   </si>
 </sst>
 </file>
@@ -87,7 +99,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -121,10 +133,52 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="0">
+        <v>269</v>
+      </c>
+      <c r="D2" s="0">
+        <v>16</v>
+      </c>
+      <c r="E2" s="0">
+        <v>15</v>
+      </c>
+      <c r="F2" s="0">
+        <v>111</v>
+      </c>
+      <c r="G2" s="0">
+        <v>110</v>
+      </c>
+      <c r="H2" s="0">
+        <v>4</v>
+      </c>
+      <c r="I2" s="0">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0">
+        <v>0</v>
+      </c>
+      <c r="L2" s="0">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
orden de las listas
</commit_message>
<xml_diff>
--- a/bin/Debug/net6.0/Resultados.xlsx
+++ b/bin/Debug/net6.0/Resultados.xlsx
@@ -23,16 +23,16 @@
     <t>Cantidad de Votantes</t>
   </si>
   <si>
+    <t>CONSENSO FEDERAL</t>
+  </si>
+  <si>
     <t>FRENTE DE IZQUIERDA Y DE TRABAJADORES - UNIDAD</t>
   </si>
   <si>
-    <t>CONSENSO FEDERAL</t>
+    <t>FRENTE DE TODOS</t>
   </si>
   <si>
     <t>JUNTOS POR EL CAMBIO</t>
-  </si>
-  <si>
-    <t>FRENTE DE TODOS</t>
   </si>
   <si>
     <t>UNITE POR LA LIBERTAD Y LA DIGNIDAD</t>
@@ -99,7 +99,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -131,15 +131,30 @@
         <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>11</v>
       </c>
     </row>
@@ -154,30 +169,45 @@
         <v>269</v>
       </c>
       <c r="D2" s="0">
+        <v>15</v>
+      </c>
+      <c r="E2" s="0">
         <v>16</v>
       </c>
-      <c r="E2" s="0">
+      <c r="F2" s="0">
+        <v>110</v>
+      </c>
+      <c r="G2" s="0">
+        <v>111</v>
+      </c>
+      <c r="H2" s="0">
+        <v>4</v>
+      </c>
+      <c r="I2" s="0">
         <v>15</v>
       </c>
-      <c r="F2" s="0">
+      <c r="J2" s="0">
+        <v>16</v>
+      </c>
+      <c r="K2" s="0">
+        <v>110</v>
+      </c>
+      <c r="L2" s="0">
         <v>111</v>
       </c>
-      <c r="G2" s="0">
-        <v>110</v>
-      </c>
-      <c r="H2" s="0">
-        <v>4</v>
-      </c>
-      <c r="I2" s="0">
-        <v>0</v>
-      </c>
-      <c r="J2" s="0">
-        <v>0</v>
-      </c>
-      <c r="K2" s="0">
-        <v>0</v>
-      </c>
-      <c r="L2" s="0">
+      <c r="M2" s="0">
+        <v>4</v>
+      </c>
+      <c r="N2" s="0">
+        <v>0</v>
+      </c>
+      <c r="O2" s="0">
+        <v>0</v>
+      </c>
+      <c r="P2" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="0">
         <v>13</v>
       </c>
     </row>

</xml_diff>